<commit_message>
added initial planning, the CDM. updated jdb
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -71,6 +71,33 @@
   </si>
   <si>
     <t>Somme de temps (h)</t>
+  </si>
+  <si>
+    <t>Gestion</t>
+  </si>
+  <si>
+    <t>Prise en connaissance du cahier des charges et entretien avec M. Gruaz</t>
+  </si>
+  <si>
+    <t>Réalisation de la planification initiale + génération d'un pdf</t>
+  </si>
+  <si>
+    <t>Relecture du cahier des charges et ajout de questions en commentaire.</t>
+  </si>
+  <si>
+    <t>Implémentation</t>
+  </si>
+  <si>
+    <t>Entretien avec Nicolas Glassey pour éclaircir le cahier des charges.</t>
+  </si>
+  <si>
+    <t>Modification de la planification initiale + génération d'un pdf</t>
+  </si>
+  <si>
+    <t>Analyse préliminaire - Introduction</t>
+  </si>
+  <si>
+    <t>Modification du MCD pour l'adapter au TPI</t>
   </si>
 </sst>
 </file>
@@ -583,6 +610,7 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="1"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -597,6 +625,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-19F0-42A4-9511-5FF83C48B94E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -612,6 +645,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-19F0-42A4-9511-5FF83C48B94E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -627,12 +665,37 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-19F0-42A4-9511-5FF83C48B94E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3EA1-4455-88CC-F97EE21D86DE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$F$11:$F$13</c:f>
+              <c:f>Feuil1!$G$11:$G$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Analyse</c:v>
                 </c:pt>
@@ -640,25 +703,31 @@
                   <c:v>Conception</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Réalisation</c:v>
+                  <c:v>Implémentation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gestion</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$11:$G$13</c:f>
+              <c:f>Feuil1!$H$11:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,16 +1389,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>246531</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>141194</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>750794</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>448237</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>26894</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123263</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1352,25 +1421,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MAITRE Nicolas" refreshedDate="43587.389011458334" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43593.373904398148" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:C43" sheet="Feuil1"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="temps (h)" numFmtId="2">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="4">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="2"/>
     </cacheField>
     <cacheField name="type" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
+      <sharedItems containsBlank="1" count="6">
+        <s v="Gestion"/>
         <s v="Analyse"/>
+        <m/>
+        <s v="Réalisation"/>
         <s v="Conception"/>
-        <s v="Réalisation"/>
-        <m/>
+        <s v="Implémentation" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1385,191 +1451,185 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="41">
   <r>
+    <n v="1"/>
     <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.75"/>
     <x v="0"/>
   </r>
   <r>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1"/>
     <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
+    <n v="2"/>
     <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <m/>
     <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <x v="4"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I29:J33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F23:G27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
-    <pivotField dataField="1" showAll="0">
-      <items count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
+      <items count="7">
+        <item x="1"/>
+        <item x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item h="1" x="3"/>
+        <item m="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1585,7 +1645,7 @@
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1875,7 +1935,7 @@
   <dimension ref="A1:AMK67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,8 +1945,8 @@
     <col min="3" max="3" width="15.42578125" style="13" customWidth="1"/>
     <col min="4" max="4" width="66.28515625" style="11" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="8"/>
-    <col min="6" max="6" width="20.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="19" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21" style="8" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="8" customWidth="1"/>
     <col min="8" max="9" width="21" style="8" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" style="8" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" style="8" customWidth="1"/>
@@ -1896,7 +1956,7 @@
     <col min="1026" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -1920,325 +1980,348 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
+        <v>43592</v>
+      </c>
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="22">
-        <v>23</v>
-      </c>
       <c r="C3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
-        <v>2</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
       <c r="B4" s="26">
         <v>2</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
-        <v>3</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
       <c r="B5" s="26">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
-        <v>4</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
       <c r="B6" s="26">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="28"/>
+        <v>13</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="42" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="43" t="str">
         <f>CONCATENATE(SUM(B3:B43), " heures")</f>
-        <v>30 heures</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8,25 heures</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="26">
+        <v>1</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>43593</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="26">
+        <v>2</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="41"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="38"/>
       <c r="C10" s="39"/>
       <c r="D10" s="40"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="26"/>
       <c r="C11" s="27"/>
       <c r="D11" s="28"/>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="8">
-        <f>GETPIVOTDATA("temps (h)",$I$29,"type","Analyse")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="8">
+        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Analyse")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="27"/>
       <c r="D12" s="28"/>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="8">
-        <f>GETPIVOTDATA("temps (h)",$I$29,"type","Conception")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="8">
+        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Conception")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="26"/>
       <c r="C13" s="27"/>
       <c r="D13" s="28"/>
-      <c r="F13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="8">
-        <f>GETPIVOTDATA("temps (h)",$I$29,"type","Réalisation")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="8" t="e">
+        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Implémentation")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="26"/>
       <c r="C14" s="27"/>
       <c r="D14" s="28"/>
       <c r="E14" s="41"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="8">
+        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Gestion")</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="26"/>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
       <c r="E16" s="41"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="26"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
       <c r="D20" s="28"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
       <c r="D21" s="28"/>
       <c r="E21" s="41"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
       <c r="D22" s="28"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
       <c r="D23" s="28"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27"/>
       <c r="D24" s="28"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="26"/>
       <c r="C25" s="27"/>
       <c r="D25" s="28"/>
+      <c r="F25" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="46"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="26"/>
       <c r="C26" s="27"/>
       <c r="D26" s="28"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
-      <c r="J26"/>
-      <c r="K26"/>
+      <c r="F26" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="46">
+        <v>2.25</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26"/>
       <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
       <c r="D27" s="28"/>
       <c r="E27" s="41"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
-      <c r="J27"/>
-      <c r="K27"/>
+      <c r="F27" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="46">
+        <v>8.25</v>
+      </c>
       <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="26"/>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="46"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
       <c r="E29" s="41"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="26"/>
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
       <c r="E30" s="41"/>
-      <c r="I30" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30" s="46">
-        <v>3</v>
-      </c>
-      <c r="K30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="26"/>
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
-      <c r="I31" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" s="46">
-        <v>2</v>
-      </c>
-      <c r="K31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="26"/>
       <c r="C32" s="27"/>
       <c r="D32" s="28"/>
-      <c r="I32" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="46">
-        <v>3</v>
-      </c>
-      <c r="K32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="26"/>
       <c r="C33" s="27"/>
       <c r="D33" s="28"/>
+      <c r="G33"/>
       <c r="H33"/>
-      <c r="I33" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="46">
-        <v>8</v>
-      </c>
-      <c r="K33"/>
+      <c r="I33"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="26"/>
       <c r="C34" s="27"/>
       <c r="D34" s="28"/>
+      <c r="G34"/>
+      <c r="H34"/>
       <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="26"/>
       <c r="C35" s="27"/>
       <c r="D35" s="28"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
@@ -2309,7 +2392,9 @@
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
       <c r="B42" s="32"/>
-      <c r="C42" s="30"/>
+      <c r="C42" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="D42" s="31"/>
       <c r="H42"/>
       <c r="I42"/>
@@ -2319,7 +2404,9 @@
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="33"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
+      <c r="C43" s="35" t="s">
+        <v>4</v>
+      </c>
       <c r="D43" s="36"/>
       <c r="H43"/>
       <c r="I43"/>

</xml_diff>

<commit_message>
Maquette création de groupe
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Préparation du rendu hebdomadaire</t>
+  </si>
+  <si>
+    <t>Finition de l'analyse préliminaire.</t>
+  </si>
+  <si>
+    <t>Modification de la maquette de la fenêtre de création de groupes.</t>
   </si>
 </sst>
 </file>
@@ -893,7 +899,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.25</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -1596,7 +1602,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43595.623269675925" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43599.346592245369" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:C43" sheet="Feuil1"/>
   </cacheSource>
@@ -1702,8 +1708,8 @@
     <x v="0"/>
   </r>
   <r>
-    <m/>
-    <x v="4"/>
+    <n v="0.25"/>
+    <x v="1"/>
   </r>
   <r>
     <m/>
@@ -1793,7 +1799,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F23:G28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -2112,8 +2118,8 @@
   </sheetPr>
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,7 +2221,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>CONCATENATE(SUM(B3:B43), " heures")</f>
-        <v>20 heures</v>
+        <v>20,5 heures</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2293,7 +2299,7 @@
       </c>
       <c r="H11" s="8">
         <f>GETPIVOTDATA("temps (h)",$F$23,"type","Analyse")</f>
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2433,29 +2439,43 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="20">
+      <c r="A21" s="45"/>
+      <c r="B21" s="46">
         <v>0.5</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="48" t="s">
         <v>32</v>
       </c>
       <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
+      <c r="A22" s="52">
+        <v>43599</v>
+      </c>
+      <c r="B22" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="F23" s="36" t="s">
         <v>9</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>8</v>
       </c>
       <c r="G24" s="38">
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2530,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="38">
-        <v>20</v>
+        <v>20.25</v>
       </c>
       <c r="I28"/>
     </row>

</xml_diff>

<commit_message>
updated sql scripts + design
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="15" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>Modification de la maquette de la fenêtre de création de groupes.</t>
+  </si>
+  <si>
+    <t>Création de la maquette de la fenêtre de chargement d'image.</t>
+  </si>
+  <si>
+    <t>Ajout de checklists dans trello.</t>
+  </si>
+  <si>
+    <t>Réalisation de la partie "conception" de l'API</t>
+  </si>
+  <si>
+    <t>Réalisation et mise à jour du MLD.</t>
+  </si>
+  <si>
+    <t>Modification du script de la base de données.</t>
   </si>
 </sst>
 </file>
@@ -872,6 +887,63 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$G$11:$G$14</c:f>
@@ -902,13 +974,13 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.75</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1602,7 +1674,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43599.346592245369" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43599.57023946759" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:C43" sheet="Feuil1"/>
   </cacheSource>
@@ -1712,28 +1784,28 @@
     <x v="1"/>
   </r>
   <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
+    <n v="0.25"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="0.25"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="0.75"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="0.5"/>
+    <x v="2"/>
   </r>
   <r>
     <m/>
@@ -1799,7 +1871,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F23:G28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -2118,8 +2190,8 @@
   </sheetPr>
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,7 +2293,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>CONCATENATE(SUM(B3:B43), " heures")</f>
-        <v>20,5 heures</v>
+        <v>24 heures</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2318,7 +2390,7 @@
       </c>
       <c r="H12" s="8">
         <f>GETPIVOTDATA("temps (h)",$F$23,"type","Conception")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2337,7 +2409,7 @@
       </c>
       <c r="H13" s="8">
         <f>GETPIVOTDATA("temps (h)",$F$23,"type","Implémentation")</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2357,7 +2429,7 @@
       </c>
       <c r="H14" s="8">
         <f>GETPIVOTDATA("temps (h)",$F$23,"type","Gestion")</f>
-        <v>2.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2466,7 +2538,10 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="55" t="str">
+        <f>CONCATENATE(SUM(B22:B28), " heures")</f>
+        <v>4 heures</v>
+      </c>
       <c r="B23" s="20">
         <v>0.25</v>
       </c>
@@ -2485,9 +2560,15 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="20">
+        <v>1</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>35</v>
+      </c>
       <c r="F24" s="37" t="s">
         <v>8</v>
       </c>
@@ -2497,62 +2578,80 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
+      <c r="B25" s="57">
+        <v>0.25</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="F25" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G25" s="38">
-        <v>3</v>
-      </c>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
+        <v>6</v>
+      </c>
       <c r="K25"/>
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="20">
+        <v>1</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="F26" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="38">
-        <v>2.75</v>
-      </c>
-      <c r="H26"/>
-      <c r="I26"/>
+        <v>3</v>
+      </c>
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
+      <c r="B27" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="E27" s="33"/>
       <c r="F27" s="37" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="38">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="42"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="F28" s="37" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="38">
-        <v>20.25</v>
-      </c>
-      <c r="I28"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="42"/>
@@ -2562,7 +2661,6 @@
       <c r="E29" s="33"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="I29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
@@ -2570,7 +2668,6 @@
       <c r="C30" s="21"/>
       <c r="D30" s="22"/>
       <c r="E30" s="33"/>
-      <c r="I30"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
@@ -2578,8 +2675,6 @@
       <c r="C31" s="21"/>
       <c r="D31" s="22"/>
       <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
@@ -2588,8 +2683,6 @@
       <c r="D32" s="22"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>

</xml_diff>

<commit_message>
update doc (analyse + conception) & fixed MLD
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="3" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Gestion externe au TPI</t>
+  </si>
+  <si>
+    <t>Ecriture de l'analyse (Utilisateurs, Conversations privées, Groupes, Messages)</t>
+  </si>
+  <si>
+    <t>Ecriture de la conception de l'API.</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -1689,7 +1695,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43600.383625115741" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43600.445378935183" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:C43" sheet="Feuil1"/>
   </cacheSource>
@@ -1843,7 +1849,7 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="0.75"/>
+    <n v="1.25"/>
     <x v="3"/>
   </r>
   <r>
@@ -1886,7 +1892,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F23:G28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -2205,8 +2211,8 @@
   </sheetPr>
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +2314,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>CONCATENATE(SUM(B3:B43), " heures")</f>
-        <v>28,25 heures</v>
+        <v>30,5 heures</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2405,7 +2411,7 @@
       </c>
       <c r="H12" s="8">
         <f>GETPIVOTDATA("temps (h)",$F$23,"type","Conception")</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,7 +2612,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="38">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
@@ -2665,7 +2671,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="38">
-        <v>27.75</v>
+        <v>28.25</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2743,7 +2749,7 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="55" t="str">
         <f>CONCATENATE(SUM(B33:B43), " heures")</f>
-        <v>1,5 heures</v>
+        <v>3,75 heures</v>
       </c>
       <c r="B34" s="20">
         <v>1.25</v>
@@ -2758,17 +2764,29 @@
       <c r="H34"/>
       <c r="I34"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="42"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
+      <c r="B35" s="20">
+        <v>1.25</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="42"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22"/>
+      <c r="B36" s="20">
+        <v>1</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>

</xml_diff>

<commit_message>
documentation update: Analyse + Conception API
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -15,9 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
-  <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -61,15 +58,6 @@
     <t>Analyse</t>
   </si>
   <si>
-    <t>Étiquettes de lignes</t>
-  </si>
-  <si>
-    <t>Total général</t>
-  </si>
-  <si>
-    <t>Somme de temps (h)</t>
-  </si>
-  <si>
     <t>Gestion</t>
   </si>
   <si>
@@ -173,6 +161,27 @@
   </si>
   <si>
     <t>Ecriture de la conception de l'API.</t>
+  </si>
+  <si>
+    <t>Continuation de la conception de l'API.</t>
+  </si>
+  <si>
+    <t>Début de l'analyse des types de données.</t>
+  </si>
+  <si>
+    <t>Début de la conception de la base de données.</t>
+  </si>
+  <si>
+    <t>Ajout de la gestion des types MIMES.</t>
+  </si>
+  <si>
+    <t>Début de la création de l'API. Création de l'architecture d'appel des méthodes / normalisation des paramètres.</t>
+  </si>
+  <si>
+    <t>Ajout de la gestion du body dans les requêtes http.</t>
+  </si>
+  <si>
+    <t>Réalisation de la méthode "getMessages", permettant de récupérer des messages dans un groupe.</t>
   </si>
 </sst>
 </file>
@@ -232,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -509,15 +518,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -611,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -716,7 +716,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -736,34 +735,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -772,7 +768,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -967,7 +963,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$G$11:$G$14</c:f>
+              <c:f>Feuil1!$G$16:$G$19</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -987,18 +983,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$H$11:$H$14</c:f>
+              <c:f>Feuil1!$H$16:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.25</c:v>
@@ -1663,16 +1659,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>750794</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>123263</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>67237</xdr:rowOff>
+      <xdr:colOff>161363</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>143437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1692,255 +1688,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="MAITRE Nicolas" refreshedDate="43600.445378935183" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="B2:C43" sheet="Feuil1"/>
-  </cacheSource>
-  <cacheFields count="2">
-    <cacheField name="temps (h)" numFmtId="2">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2.5"/>
-    </cacheField>
-    <cacheField name="type" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
-        <s v="Gestion"/>
-        <s v="Analyse"/>
-        <s v="Implémentation"/>
-        <s v="Conception"/>
-        <m/>
-        <s v="Réalisation" u="1"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="41">
-  <r>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="0.75"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="1.5"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.75"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.75"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="2.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.75"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0.5"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0.25"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1.25"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F23:G28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
-      <items count="7">
-        <item x="1"/>
-        <item x="3"/>
-        <item h="1" m="1" x="5"/>
-        <item h="1" x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Somme de temps (h)" fld="0" baseField="1" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2211,15 +1958,15 @@
   </sheetPr>
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="40" customWidth="1"/>
     <col min="4" max="4" width="66.28515625" style="11" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="8"/>
     <col min="6" max="6" width="21" style="8" customWidth="1"/>
@@ -2237,8 +1984,8 @@
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2258,21 +2005,21 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
+      <c r="A3" s="52">
         <v>43592</v>
       </c>
       <c r="B3" s="17">
         <v>1</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="str">
+      <c r="A4" s="53" t="str">
         <f>CONCATENATE(SUM(B3:B7), " heures")</f>
         <v>5,25 heures</v>
       </c>
@@ -2283,98 +2030,98 @@
         <v>8</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="20">
         <v>0.75</v>
       </c>
       <c r="C5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="20">
         <v>0.5</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="35" t="str">
-        <f>CONCATENATE(SUM(B3:B43), " heures")</f>
-        <v>30,5 heures</v>
+        <f>CONCATENATE(SUM(B3:B54), " heures")</f>
+        <v>37,25 heures</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46">
+      <c r="A7" s="43"/>
+      <c r="B7" s="44">
         <v>1</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="48" t="s">
-        <v>18</v>
+      <c r="D7" s="46" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="53">
+      <c r="A8" s="51">
         <v>43593</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="47">
         <v>1.5</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="51" t="s">
-        <v>19</v>
+      <c r="D8" s="49" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="str">
+      <c r="A9" s="54" t="str">
         <f>CONCATENATE(SUM(B8:B9), " heures")</f>
         <v>3,5 heures</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="44">
         <v>2</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>20</v>
+      <c r="C9" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
+      <c r="A10" s="51">
         <v>43594</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="47">
         <v>2</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>21</v>
+      <c r="C10" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="str">
+      <c r="A11" s="53" t="str">
         <f>CONCATENATE(SUM(B10:B14), " heures")</f>
         <v>5,75 heures</v>
       </c>
@@ -2385,18 +2132,11 @@
         <v>8</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="8">
-        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Analyse")</f>
-        <v>7.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="20">
         <v>0.5</v>
       </c>
@@ -2404,18 +2144,11 @@
         <v>8</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="8">
-        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Conception")</f>
-        <v>7.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="20">
         <v>1</v>
       </c>
@@ -2423,52 +2156,38 @@
         <v>8</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="8">
-        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Implémentation")</f>
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="46">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44">
         <v>2</v>
       </c>
-      <c r="C14" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>25</v>
+      <c r="C14" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="33"/>
-      <c r="G14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="8">
-        <f>GETPIVOTDATA("temps (h)",$F$23,"type","Gestion")</f>
-        <v>4.25</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
+      <c r="A15" s="50">
         <v>43595</v>
       </c>
       <c r="B15" s="30">
         <v>0.75</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="str">
+      <c r="A16" s="53" t="str">
         <f>CONCATENATE(SUM(B15:B21), " heures")</f>
         <v>5,5 heures</v>
       </c>
@@ -2476,27 +2195,41 @@
         <v>0.25</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="33"/>
+      <c r="G16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="8">
+        <f>SUMIF(C$3:C$1048576,G16,B$3:B$1048576)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="20">
         <v>0.75</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" ref="H17:H19" si="0">SUMIF(C$3:C$1048576,G17,B$3:B$1048576)</f>
+        <v>9.5</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="20">
         <v>2.5</v>
       </c>
@@ -2504,48 +2237,62 @@
         <v>4</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="57">
+      <c r="A19" s="41"/>
+      <c r="B19" s="55">
         <v>0.5</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="20">
         <v>0.25</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="46">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44">
         <v>0.5</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>32</v>
+      <c r="C21" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>29</v>
       </c>
       <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="A22" s="50">
         <v>43599</v>
       </c>
       <c r="B22" s="30">
@@ -2555,11 +2302,11 @@
         <v>8</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="str">
+      <c r="A23" s="53" t="str">
         <f>CONCATENATE(SUM(B22:B32), " heures")</f>
         <v>6,75 heures</v>
       </c>
@@ -2570,17 +2317,13 @@
         <v>4</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="20">
         <v>1</v>
       </c>
@@ -2588,37 +2331,29 @@
         <v>4</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="38">
-        <v>7.5</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="57">
+      <c r="A25" s="41"/>
+      <c r="B25" s="55">
         <v>0.25</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="38">
-        <v>7.5</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
       <c r="K25"/>
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="20">
         <v>1</v>
       </c>
@@ -2626,18 +2361,14 @@
         <v>4</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="38">
-        <v>4.25</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="20">
         <v>0.75</v>
       </c>
@@ -2645,65 +2376,57 @@
         <v>4</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E27" s="33"/>
-      <c r="F27" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="38">
-        <v>9</v>
-      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="20">
         <v>0.5</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="38">
-        <v>28.25</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="20">
         <v>0.5</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E29" s="33"/>
       <c r="F29"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="20">
         <v>1</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="20">
         <v>1</v>
       </c>
@@ -2711,44 +2434,44 @@
         <v>8</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
-      <c r="B32" s="46">
+      <c r="A32" s="43"/>
+      <c r="B32" s="44">
         <v>0.25</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="48" t="s">
-        <v>42</v>
+      <c r="D32" s="46" t="s">
+        <v>39</v>
       </c>
       <c r="F32"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="52">
+      <c r="A33" s="50">
         <v>43600</v>
       </c>
       <c r="B33" s="30">
         <v>0.25</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="str">
-        <f>CONCATENATE(SUM(B33:B43), " heures")</f>
+      <c r="A34" s="53" t="str">
+        <f>CONCATENATE(SUM(B33:B36), " heures")</f>
         <v>3,75 heures</v>
       </c>
       <c r="B34" s="20">
@@ -2758,14 +2481,14 @@
         <v>4</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="20">
         <v>1.25</v>
       </c>
@@ -2773,38 +2496,55 @@
         <v>8</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="20">
+      <c r="A36" s="43"/>
+      <c r="B36" s="44">
         <v>1</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="22" t="s">
-        <v>46</v>
+      <c r="D36" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="50">
+        <v>43601</v>
+      </c>
+      <c r="B37" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>44</v>
+      </c>
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
+      <c r="A38" s="53" t="str">
+        <f>CONCATENATE(SUM(B37:B47), " heures")</f>
+        <v>6,75 heures</v>
+      </c>
+      <c r="B38" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -2813,10 +2553,16 @@
       <c r="M38"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -2825,10 +2571,16 @@
       <c r="M39"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="22"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -2836,11 +2588,17 @@
       <c r="L40"/>
       <c r="M40"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="22"/>
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="41"/>
+      <c r="B41" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
@@ -2849,153 +2607,177 @@
       <c r="M41"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="26">
+        <v>1</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>49</v>
+      </c>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="43"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="B43" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C44" s="6"/>
-      <c r="D44" s="44"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="25"/>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="4"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="25"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="4"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="25"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="4"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="25"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="4"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="25"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="4"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="41"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="25"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="4"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="41"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="25"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="4"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="41"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="25"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="4"/>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="25"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="41"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="42"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="29"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="1"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="1"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="1"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="1"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="1"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="1"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="1"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="1"/>
       <c r="D64" s="4"/>
@@ -3014,7 +2796,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" scale="83" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update doc + jdt
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -182,6 +182,27 @@
   </si>
   <si>
     <t>Réalisation de la méthode "getMessages", permettant de récupérer des messages dans un groupe.</t>
+  </si>
+  <si>
+    <t>Résolution des bugs d'envoi de message en préparation de l'entretien de mardi.</t>
+  </si>
+  <si>
+    <t>Finition de la création de la méthode "getMessages" sur l'API</t>
+  </si>
+  <si>
+    <t>Création de méthodes de contact de la base de données depuis le client web.</t>
+  </si>
+  <si>
+    <t>Création de la méthode getUser sur l'API.</t>
+  </si>
+  <si>
+    <t>Modification des appels hardcodés existant pour utiliser l'API.</t>
+  </si>
+  <si>
+    <t>Création de la méthode getGroups sur l'API.</t>
+  </si>
+  <si>
+    <t>Création d'une page d'erreur.</t>
   </si>
 </sst>
 </file>
@@ -611,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -773,6 +794,24 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,7 +1033,7 @@
                   <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.5</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.25</c:v>
@@ -1958,8 +1997,8 @@
   </sheetPr>
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2100,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>CONCATENATE(SUM(B3:B54), " heures")</f>
-        <v>37,25 heures</v>
+        <v>42,5 heures</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2244,7 +2283,7 @@
       </c>
       <c r="H18" s="8">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2533,7 +2572,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="str">
-        <f>CONCATENATE(SUM(B37:B47), " heures")</f>
+        <f>CONCATENATE(SUM(B37:B43), " heures")</f>
         <v>6,75 heures</v>
       </c>
       <c r="B38" s="23">
@@ -2623,14 +2662,14 @@
       <c r="K42"/>
     </row>
     <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="26">
+      <c r="A43" s="43"/>
+      <c r="B43" s="59">
         <v>0.5</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="61" t="s">
         <v>50</v>
       </c>
       <c r="H43"/>
@@ -2638,31 +2677,54 @@
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="25"/>
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="50">
+        <v>43602</v>
+      </c>
+      <c r="B44" s="56">
+        <v>0.75</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>51</v>
+      </c>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="25"/>
+      <c r="A45" s="53" t="str">
+        <f>CONCATENATE(SUM(B44:B50), " heures")</f>
+        <v>5,25 heures</v>
+      </c>
+      <c r="B45" s="26">
+        <v>0.75</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="41"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
+      <c r="B46" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
@@ -2670,36 +2732,60 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="41"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="25"/>
+      <c r="B47" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="41"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="25"/>
+      <c r="B48" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="41"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="25"/>
+      <c r="B49" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
+      <c r="B50" s="26">
+        <v>1</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>

</xml_diff>

<commit_message>
update db_creation script + update doc
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -302,6 +302,21 @@
   </si>
   <si>
     <t>Entretien avec M. Glassey.</t>
+  </si>
+  <si>
+    <t>Remplissage du journal de travail et trello.</t>
+  </si>
+  <si>
+    <t>Réalisation de la section "Contexte"</t>
+  </si>
+  <si>
+    <t>Ajout de css pour changer la taille de la fenêtre.</t>
+  </si>
+  <si>
+    <t>Conception de la FilesAPI</t>
+  </si>
+  <si>
+    <t>Création de la FilesAPI: endpoint + default data</t>
   </si>
 </sst>
 </file>
@@ -984,25 +999,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="8"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1017,12 +1028,23 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1075,6 +1097,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C6500"/>
       </font>
@@ -1095,48 +1134,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1403,16 +1400,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.75</c:v>
+                  <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
@@ -2379,8 +2376,8 @@
   </sheetPr>
   <dimension ref="A1:AMK154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2479,7 +2476,7 @@
       </c>
       <c r="G6" s="55">
         <f>SUM(B3:B144)</f>
-        <v>69.5</v>
+        <v>73.25</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>76</v>
@@ -2525,7 +2522,7 @@
       </c>
       <c r="G8" s="54">
         <f>G7-G6</f>
-        <v>-2</v>
+        <v>-5.75</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>76</v>
@@ -2916,7 +2913,7 @@
       </c>
       <c r="G24" s="3">
         <f>SUMIF(C$3:C$1048576,F24,B$3:B$1048576)</f>
-        <v>10.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -2935,7 +2932,7 @@
       </c>
       <c r="G25" s="3">
         <f>SUMIF(C$3:C$1048576,F25,B$3:B$1048576)</f>
-        <v>21.75</v>
+        <v>22.25</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
@@ -2956,7 +2953,7 @@
       </c>
       <c r="G26" s="3">
         <f>SUMIF(C$3:C$1048576,F26,B$3:B$1048576) +N("Rien n'est truqué absolument pas du tout")</f>
-        <v>29</v>
+        <v>31.25</v>
       </c>
       <c r="L26"/>
     </row>
@@ -2977,7 +2974,7 @@
       </c>
       <c r="G27" s="3">
         <f>SUMIF(C$3:C$1048576,F27,B$3:B$1048576)</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="L27"/>
     </row>
@@ -3641,8 +3638,8 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="43" t="str">
-        <f>CONCATENATE(SUM(B71:B77), " heures")</f>
-        <v>5,25 heures</v>
+        <f>CONCATENATE(SUM(B71:B78), " heures")</f>
+        <v>6,75 heures</v>
       </c>
       <c r="B72" s="21">
         <v>0.25</v>
@@ -3704,7 +3701,9 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="43"/>
-      <c r="B77" s="21"/>
+      <c r="B77" s="21">
+        <v>1</v>
+      </c>
       <c r="C77" s="19" t="s">
         <v>13</v>
       </c>
@@ -3713,46 +3712,81 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="43"/>
-      <c r="B78" s="21">
+      <c r="A78" s="44"/>
+      <c r="B78" s="49">
         <v>0.5</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D78" s="20" t="s">
+      <c r="D78" s="51" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="43"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="20"/>
+      <c r="A79" s="40">
+        <v>43614</v>
+      </c>
+      <c r="B79" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="48" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="43"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="20"/>
+      <c r="A80" s="43" t="str">
+        <f>CONCATENATE(SUM(B79:B85), " heures")</f>
+        <v>2,75 heures</v>
+      </c>
+      <c r="B80" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="43"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="20"/>
+      <c r="B81" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="43"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="20"/>
+      <c r="B82" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="43"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="20"/>
+      <c r="B83" s="21">
+        <v>1</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="43"/>
@@ -3845,24 +3879,64 @@
       <c r="R154" s="60"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+  <conditionalFormatting sqref="C1:C78 C81:C82 C84:C1048576">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>$F$25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>$F$26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>$F$27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>$F$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>$F$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:C80">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>$F$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>$F$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>$F$27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>$F$26</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>$F$25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>$F$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$F$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>$F$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>$F$27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>$F$26</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>$F$25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update doc +  default data
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>Création de la FilesAPI: endpoint + default data</t>
+  </si>
+  <si>
+    <t>Résolution d'un souci lors d'un merge sur git</t>
+  </si>
+  <si>
+    <t>Envoi d'un email aux experts (+Nicolas Glassey)</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1009,31 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1018,19 +1048,16 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="8"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1044,14 +1071,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="8"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,33 +1096,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1362,9 +1368,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1409,7 +1413,7 @@
                   <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
@@ -1447,7 +1451,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2377,7 +2380,7 @@
   <dimension ref="A1:AMK154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,7 +2479,7 @@
       </c>
       <c r="G6" s="55">
         <f>SUM(B3:B144)</f>
-        <v>73.25</v>
+        <v>74.25</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>76</v>
@@ -2522,7 +2525,7 @@
       </c>
       <c r="G8" s="54">
         <f>G7-G6</f>
-        <v>-5.75</v>
+        <v>-6.75</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>76</v>
@@ -2974,7 +2977,7 @@
       </c>
       <c r="G27" s="3">
         <f>SUMIF(C$3:C$1048576,F27,B$3:B$1048576)</f>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="L27"/>
     </row>
@@ -3740,7 +3743,7 @@
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="43" t="str">
         <f>CONCATENATE(SUM(B79:B85), " heures")</f>
-        <v>2,75 heures</v>
+        <v>3,75 heures</v>
       </c>
       <c r="B80" s="21">
         <v>0.5</v>
@@ -3790,15 +3793,27 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="43"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="20"/>
+      <c r="B84" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="43"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="20"/>
+      <c r="B85" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="43"/>
@@ -3900,42 +3915,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C80">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>$F$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$F$27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>$F$26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>$F$25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$F$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$F$27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>$F$26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$F$25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
upadte doc + résumé + group creation procedure
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2280" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2280" windowHeight="6615" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="108">
   <si>
     <t>Nicolas Maitre</t>
   </si>
@@ -323,6 +323,36 @@
   </si>
   <si>
     <t>Envoi d'un email aux experts (+Nicolas Glassey)</t>
+  </si>
+  <si>
+    <t>Aide à un camarade, requête sql sur deux tables séparées par deux tables intermédiaires. Utile pour la résupération des utilisateurs de l'application.</t>
+  </si>
+  <si>
+    <t>Création du résumé du TPI.</t>
+  </si>
+  <si>
+    <t>Création de la fenêtre de création de groupes.</t>
+  </si>
+  <si>
+    <t>Création de l'endpoint "getUsers" dans l'API</t>
+  </si>
+  <si>
+    <t>Création de la liste des users dans la fenêtre de création de groupe</t>
+  </si>
+  <si>
+    <t>Création de l'action "addGroup" dans le WebSocket (serveur)</t>
+  </si>
+  <si>
+    <t>Création de l'action "newGroup" dans le WebSocket (client)</t>
+  </si>
+  <si>
+    <t>Remplissage du journal de bord</t>
+  </si>
+  <si>
+    <t>Correction de bugs dans l'ajout de groupes</t>
+  </si>
+  <si>
+    <t>Mise à jour des issues</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1135,31 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1120,33 +1174,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1410,16 +1440,16 @@
                   <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.25</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2377,10 +2407,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK154"/>
+  <dimension ref="A1:AMK156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,8 +2508,8 @@
         <v>6</v>
       </c>
       <c r="G6" s="55">
-        <f>SUM(B3:B144)</f>
-        <v>74.25</v>
+        <f>SUM(B3:B146)</f>
+        <v>83.5</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>76</v>
@@ -2500,8 +2530,7 @@
         <v>74</v>
       </c>
       <c r="G7" s="3">
-        <f>3*22.5</f>
-        <v>67.5</v>
+        <v>90</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>76</v>
@@ -2525,7 +2554,7 @@
       </c>
       <c r="G8" s="54">
         <f>G7-G6</f>
-        <v>-6.75</v>
+        <v>6.5</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>76</v>
@@ -2956,7 +2985,7 @@
       </c>
       <c r="G26" s="3">
         <f>SUMIF(C$3:C$1048576,F26,B$3:B$1048576) +N("Rien n'est truqué absolument pas du tout")</f>
-        <v>31.25</v>
+        <v>37</v>
       </c>
       <c r="L26"/>
     </row>
@@ -2977,7 +3006,7 @@
       </c>
       <c r="G27" s="3">
         <f>SUMIF(C$3:C$1048576,F27,B$3:B$1048576)</f>
-        <v>8.5</v>
+        <v>11.5</v>
       </c>
       <c r="L27"/>
     </row>
@@ -3017,7 +3046,7 @@
       </c>
       <c r="G29" s="3">
         <f>SUMIF(C$3:C$1048576,F29,B$3:B$1048576)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3804,40 +3833,236 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="43"/>
-      <c r="B85" s="21">
+      <c r="A85" s="44"/>
+      <c r="B85" s="49">
         <v>0.25</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D85" s="20" t="s">
+      <c r="D85" s="51" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="43"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="20"/>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="52"/>
-      <c r="B87" s="53"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="23"/>
-    </row>
-    <row r="139" spans="15:21" x14ac:dyDescent="0.25">
-      <c r="O139" s="59"/>
-      <c r="P139" s="59"/>
-      <c r="T139" s="59"/>
-      <c r="U139" s="59"/>
-    </row>
-    <row r="140" spans="15:21" x14ac:dyDescent="0.25">
-      <c r="O140" s="59"/>
-      <c r="P140" s="59"/>
-      <c r="T140" s="59"/>
-      <c r="U140" s="59"/>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="40">
+        <v>43620</v>
+      </c>
+      <c r="B86" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C86" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86" s="48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="43" t="str">
+        <f>CONCATENATE(SUM(B86:B92), " heures")</f>
+        <v>6,75 heures</v>
+      </c>
+      <c r="B87" s="21">
+        <v>1</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="43"/>
+      <c r="B88" s="21">
+        <v>2</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="43"/>
+      <c r="B89" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="43"/>
+      <c r="B90" s="21">
+        <v>1</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="43"/>
+      <c r="B91" s="21">
+        <v>1</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="44"/>
+      <c r="B92" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="C92" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="40">
+        <v>43621</v>
+      </c>
+      <c r="B93" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C93" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="43" t="str">
+        <f>CONCATENATE(SUM(B93:B99), " heures")</f>
+        <v>2,5 heures</v>
+      </c>
+      <c r="B94" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="43"/>
+      <c r="B95" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="43"/>
+      <c r="B96" s="21">
+        <v>1</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="43"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="20"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="43"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="20"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="43"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="20"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="43"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="20"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="43"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="20"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="43"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="20"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="43"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="20"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="43"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="20"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="43"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="20"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="43"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="20"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="43"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="20"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="43"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="20"/>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="52"/>
+      <c r="B109" s="53"/>
+      <c r="C109" s="22"/>
+      <c r="D109" s="23"/>
     </row>
     <row r="141" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O141" s="59"/>
@@ -3847,43 +4072,45 @@
     </row>
     <row r="142" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O142" s="59"/>
-      <c r="P142" s="57"/>
-      <c r="T142" s="57"/>
+      <c r="P142" s="59"/>
+      <c r="T142" s="59"/>
       <c r="U142" s="59"/>
     </row>
-    <row r="148" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N148" s="62"/>
-      <c r="V148" s="62"/>
-    </row>
-    <row r="149" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N149" s="59"/>
-      <c r="O149" s="62"/>
-      <c r="P149" s="62"/>
-      <c r="Q149" s="62"/>
-      <c r="R149" s="62"/>
-      <c r="S149" s="62"/>
-      <c r="T149" s="62"/>
-      <c r="U149" s="62"/>
-      <c r="V149" s="59"/>
+    <row r="143" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O143" s="59"/>
+      <c r="P143" s="59"/>
+      <c r="T143" s="59"/>
+      <c r="U143" s="59"/>
+    </row>
+    <row r="144" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O144" s="59"/>
+      <c r="P144" s="57"/>
+      <c r="T144" s="57"/>
+      <c r="U144" s="59"/>
     </row>
     <row r="150" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="O150" s="59"/>
-      <c r="P150" s="59"/>
-      <c r="Q150" s="60"/>
-      <c r="R150" s="61"/>
-      <c r="S150" s="60"/>
-      <c r="T150" s="59"/>
-      <c r="U150" s="59"/>
+      <c r="N150" s="62"/>
+      <c r="V150" s="62"/>
     </row>
     <row r="151" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="Q151" s="60"/>
-      <c r="R151" s="61"/>
-      <c r="S151" s="60"/>
+      <c r="N151" s="59"/>
+      <c r="O151" s="62"/>
+      <c r="P151" s="62"/>
+      <c r="Q151" s="62"/>
+      <c r="R151" s="62"/>
+      <c r="S151" s="62"/>
+      <c r="T151" s="62"/>
+      <c r="U151" s="62"/>
+      <c r="V151" s="59"/>
     </row>
     <row r="152" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="O152" s="59"/>
+      <c r="P152" s="59"/>
       <c r="Q152" s="60"/>
       <c r="R152" s="61"/>
       <c r="S152" s="60"/>
+      <c r="T152" s="59"/>
+      <c r="U152" s="59"/>
     </row>
     <row r="153" spans="14:22" x14ac:dyDescent="0.25">
       <c r="Q153" s="60"/>
@@ -3891,27 +4118,37 @@
       <c r="S153" s="60"/>
     </row>
     <row r="154" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="R154" s="60"/>
+      <c r="Q154" s="60"/>
+      <c r="R154" s="61"/>
+      <c r="S154" s="60"/>
+    </row>
+    <row r="155" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="Q155" s="60"/>
+      <c r="R155" s="61"/>
+      <c r="S155" s="60"/>
+    </row>
+    <row r="156" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="R156" s="60"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C78 C81:C82 C84:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
-      <formula>$F$24</formula>
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>$F$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>$F$27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>$F$26</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>$F$25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>$F$26</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>$F$27</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>$F$29</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
-      <formula>$F$28</formula>
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+      <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C80">

</xml_diff>